<commit_message>
fix: resolve #1 - correct selector for Instagram message typing
</commit_message>
<xml_diff>
--- a/Instgram_Output_File.xlsx
+++ b/Instgram_Output_File.xlsx
@@ -44,10 +44,10 @@
     <x:t>SentComment</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.instagram.com/delinda.gucwa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Belaliet Houssame Eddine</x:t>
+    <x:t>https://www.instagram.com/oldrich.hanak.3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hex ️</x:t>
   </x:si>
   <x:si>
     <x:t>Skip</x:t>

</xml_diff>

<commit_message>
Fix, Resolve #7 Adjust Comment Precondition to be in Comment Case and Both only
</commit_message>
<xml_diff>
--- a/Instgram_Output_File.xlsx
+++ b/Instgram_Output_File.xlsx
@@ -47,10 +47,7 @@
     <x:t>ChromeProfile</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.instagram.com/kloxyfn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>oliver haavisto</x:t>
+    <x:t>https://www.instagram.com/b00nd0xkhg</x:t>
   </x:si>
   <x:si>
     <x:t>Skip</x:t>
@@ -435,17 +432,14 @@
       <x:c r="A2" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>